<commit_message>
COMMIT_DL_DOMICILE apres questions à traiter
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="102">
   <si>
     <t>Version utilisée</t>
   </si>
@@ -434,9 +434,6 @@
     <t>ORM (object-relational mapping)</t>
   </si>
   <si>
-    <t>Hibernate</t>
-  </si>
-  <si>
     <t>5.2.10.Final</t>
   </si>
   <si>
@@ -453,12 +450,114 @@
   </si>
   <si>
     <t>1.2</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/javax.validation/validation-api/2.0.0.Final</t>
+  </si>
+  <si>
+    <t>Validation de formulaires Web</t>
+  </si>
+  <si>
+    <t>2.0.0.Final</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.hibernate/hibernate-validator/6.0.1.Final</t>
+  </si>
+  <si>
+    <t>6.0.1.Final</t>
+  </si>
+  <si>
+    <t>Bean Validation API 2.0.0.Final</t>
+  </si>
+  <si>
+    <t>Hibernate Validator 6.0.1.Final</t>
+  </si>
+  <si>
+    <t>Modélisation</t>
+  </si>
+  <si>
+    <t>Enterprise Architect 13.5.1351 (32 bits)</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.hibernate.javax.persistence/hibernate-jpa-2.1-api/1.0.0.Final</t>
+  </si>
+  <si>
+    <t>1.0.0.Final</t>
+  </si>
+  <si>
+    <t>Java Persistence API - Entity Manager</t>
+  </si>
+  <si>
+    <t>JPA 2.1 (hibernate-jpa-2.1-api-1.0.0.Final-sources.jar)</t>
+  </si>
+  <si>
+    <t>Jboss Hibernate (Hibernate-core5.2.10.Final)</t>
+  </si>
+  <si>
+    <t>UML 2.0</t>
+  </si>
+  <si>
+    <t>5.7.19</t>
+  </si>
+  <si>
+    <t>Oracle MySQL Server 5.7.19</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/mysql/mysql-connector-java/8.0.7-dmr</t>
+  </si>
+  <si>
+    <t>https://dev.mysql.com/downloads/windows/installer/5.7.html</t>
+  </si>
+  <si>
+    <t>MySQL Connector/J  8.0.7-dmr</t>
+  </si>
+  <si>
+    <t>8.0.7-dmr</t>
+  </si>
+  <si>
+    <t>13.5.1351</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  http://www.omg.org/spec/UML/2.0</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>PostgreSQL 9.6.4</t>
+  </si>
+  <si>
+    <t>https://www.enterprisedb.com/downloads/postgres-postgresql-downloads#windows</t>
+  </si>
+  <si>
+    <t>9.6.4</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/postgresql/postgresql/9.1-901-1.jdbc4</t>
+  </si>
+  <si>
+    <t>PostgreSQL JDBC Driver 9.1-901-1.jdbc4</t>
+  </si>
+  <si>
+    <t>9.1-901-1.jdbc4</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.tomcat/tomcat-servlet-api/8.5.11</t>
+  </si>
+  <si>
+    <t>9.0.0.M26</t>
+  </si>
+  <si>
+    <t>Apache Tomcat 8.5.12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -861,11 +960,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -924,7 +1023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
@@ -941,7 +1040,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1026,198 +1125,389 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="10"/>
-      <c r="D11" s="3"/>
-    </row>
     <row r="12" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="10"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s">
+    <row r="14" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="10"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="10"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="10"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="10"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="10"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="10"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="10"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+    <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C32" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="10"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D7" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D8" r:id="rId5"/>
-    <hyperlink ref="D9" r:id="rId6"/>
-    <hyperlink ref="D10" r:id="rId7"/>
-    <hyperlink ref="D19" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
-    <hyperlink ref="D22" r:id="rId10"/>
-    <hyperlink ref="D26" r:id="rId11"/>
-    <hyperlink ref="D14" r:id="rId12"/>
-    <hyperlink ref="D12" r:id="rId13"/>
-    <hyperlink ref="D24" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D28" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D37" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D39" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D40" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D29" r:id="rId23" xr:uid="{94B18ED3-E673-44B7-AF22-1689CBC74A92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après ajout composants Maven
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="140">
   <si>
     <t>Version utilisée</t>
   </si>
@@ -386,9 +386,6 @@
     <t>Serveur applicatif</t>
   </si>
   <si>
-    <t>Apache Tomcat 8.5.11</t>
-  </si>
-  <si>
     <t>9.0</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t>5.7.19</t>
   </si>
   <si>
-    <t>Oracle MySQL Server 5.7.19</t>
-  </si>
-  <si>
     <t>https://mvnrepository.com/artifact/mysql/mysql-connector-java/8.0.7-dmr</t>
   </si>
   <si>
@@ -527,9 +521,6 @@
     <t>2.5</t>
   </si>
   <si>
-    <t>PostgreSQL 9.6.4</t>
-  </si>
-  <si>
     <t>https://www.enterprisedb.com/downloads/postgres-postgresql-downloads#windows</t>
   </si>
   <si>
@@ -552,6 +543,129 @@
   </si>
   <si>
     <t>Apache Tomcat 8.5.12</t>
+  </si>
+  <si>
+    <t>Serveur applicatif (embarqué dans l'appli dans SpringBoot)</t>
+  </si>
+  <si>
+    <t>Serveur PostgreSQL 9.6.4</t>
+  </si>
+  <si>
+    <t>Serveur Oracle MySQL Server 5.7.19</t>
+  </si>
+  <si>
+    <t>Serveur Apache Tomcat 8.5.11</t>
+  </si>
+  <si>
+    <t>Attention, la version de Maven utilisée (embarquée) dans Eclipse peut êtrte différente</t>
+  </si>
+  <si>
+    <t>Apache Maven Compiler Plugin » 3.6.2</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-compiler-plugin/3.6.2</t>
+  </si>
+  <si>
+    <t>3.6.2</t>
+  </si>
+  <si>
+    <t>maven-antrun-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-antrun-plugin/1.8</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>maven-assembly-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-assembly-plugin/3.1.0</t>
+  </si>
+  <si>
+    <t>3.1.0</t>
+  </si>
+  <si>
+    <t>maven-dependency-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-dependency-plugin/3.0.1</t>
+  </si>
+  <si>
+    <t>3.0.1</t>
+  </si>
+  <si>
+    <t>maven-release-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-release-plugin/2.5.3</t>
+  </si>
+  <si>
+    <t>2.5.3</t>
+  </si>
+  <si>
+    <t>maven-clean-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-clean-plugin/3.0.0</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
+  </si>
+  <si>
+    <t>maven-resources-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-resources-plugin/3.0.2</t>
+  </si>
+  <si>
+    <t>3.0.2</t>
+  </si>
+  <si>
+    <t>maven-war-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-war-plugin/3.1.0</t>
+  </si>
+  <si>
+    <t>maven-compiler-plugin</t>
+  </si>
+  <si>
+    <t>maven-surefire-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-surefire-plugin/2.20</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>maven-install-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-install-plugin/2.5.2</t>
+  </si>
+  <si>
+    <t>2.5.2</t>
+  </si>
+  <si>
+    <t>maven-deploy-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-deploy-plugin/2.8.2</t>
+  </si>
+  <si>
+    <t>2.8.2</t>
+  </si>
+  <si>
+    <t>maven-site-plugin</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.maven.plugins/maven-site-plugin/3.6</t>
+  </si>
+  <si>
+    <t>3.6</t>
   </si>
 </sst>
 </file>
@@ -961,10 +1075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F43"/>
+  <dimension ref="B1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -975,10 +1089,11 @@
     <col min="4" max="4" width="74.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="54.140625" style="5" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="19.5703125" style="1"/>
+    <col min="7" max="7" width="48.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="19.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:7" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
@@ -995,7 +1110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:6" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1006,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1023,7 +1138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1040,7 +1155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:6" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
@@ -1056,8 +1171,11 @@
       <c r="F5" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1074,440 +1192,645 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="8"/>
+      <c r="E19" s="7"/>
+    </row>
+    <row r="20" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="8"/>
+      <c r="E21" s="7"/>
+    </row>
+    <row r="22" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="23" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+    <row r="24" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="25" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C27" s="10"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="10"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="3" t="s">
+    <row r="29" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="10"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="10"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C32" s="10"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="10"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="10"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="10"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="10"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="10"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="10"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="10"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="C47" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="10"/>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="10"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="10"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="25" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="10"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="D57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>89</v>
+      <c r="F58" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="D26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="D28" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D34" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="D13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D32" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="D22" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="D19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="D20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D31" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D37" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D39" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D40" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="D29" r:id="rId23" xr:uid="{94B18ED3-E673-44B7-AF22-1689CBC74A92}"/>
+    <hyperlink ref="D23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D26" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D41" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D49" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D30" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D47" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D37" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D34" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D46" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D52" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D51" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D54" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D55" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D44" r:id="rId23" xr:uid="{94B18ED3-E673-44B7-AF22-1689CBC74A92}"/>
+    <hyperlink ref="D7" r:id="rId24" xr:uid="{6CA69A82-E20A-4525-955A-629EFF7FED41}"/>
+    <hyperlink ref="D8" r:id="rId25" xr:uid="{BF5198FE-BAFA-4C0E-925F-575EE5DDF14B}"/>
+    <hyperlink ref="D9" r:id="rId26" xr:uid="{A4D64F4C-1076-45AB-98EB-5AAE371373DF}"/>
+    <hyperlink ref="D10" r:id="rId27" xr:uid="{A2E0DDCC-B7D3-4C49-AD7F-584BBFF65FBC}"/>
+    <hyperlink ref="D11" r:id="rId28" xr:uid="{049A63D1-4A5B-4D47-891F-47FD1C1516DF}"/>
+    <hyperlink ref="D12" r:id="rId29" xr:uid="{B612AFF2-C7A0-4EC6-BD16-B8EE7BBA5413}"/>
+    <hyperlink ref="D13" r:id="rId30" xr:uid="{00C1EF65-411B-4707-A73A-891E644AA18E}"/>
+    <hyperlink ref="D14" r:id="rId31" xr:uid="{11E0891A-9566-4101-9BB2-FC805FE58B2D}"/>
+    <hyperlink ref="D15" r:id="rId32" xr:uid="{C426670A-19F3-460B-9E69-B0B81143C11A}"/>
+    <hyperlink ref="D16" r:id="rId33" xr:uid="{BF214671-2269-4A56-A738-777AE0D1A23B}"/>
+    <hyperlink ref="D17" r:id="rId34" xr:uid="{2B655D3E-9F6D-4C4A-9A02-DAC1C011BC96}"/>
+    <hyperlink ref="D18" r:id="rId35" xr:uid="{21ACE2EB-4E33-453D-BA93-6881E1705DE3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après modif questions
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dan\git\traficweb_maven\configuration_de_developpement\Configuration de développement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Donnees\eclipse\eclipseworkspace_neon\traficweb_maven\configuration_de_developpement\Configuration de développement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="144">
   <si>
     <t>Version utilisée</t>
   </si>
@@ -666,6 +666,18 @@
   </si>
   <si>
     <t>3.6</t>
+  </si>
+  <si>
+    <t>Version de Servlet (Pré-requis : les conteneur de Servlet doit pouvoir gérer la version de servlet 3.1)</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/javax.servlet/javax.servlet-api/3.1.0</t>
+  </si>
+  <si>
+    <t>4.0.0</t>
+  </si>
+  <si>
+    <t>servlet-api 3.1</t>
   </si>
 </sst>
 </file>
@@ -728,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -759,6 +771,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1075,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G58"/>
+  <dimension ref="B1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1637,158 +1652,175 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
+    <row r="45" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+    <row r="50" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="10"/>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="10"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C58" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1804,18 +1836,18 @@
     <hyperlink ref="D40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="D41" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="D43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D49" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D50" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="D30" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="D47" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D48" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="D37" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="D34" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="D35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D46" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D52" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D51" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D54" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D55" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D47" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D53" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D55" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D56" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="D44" r:id="rId23" xr:uid="{94B18ED3-E673-44B7-AF22-1689CBC74A92}"/>
     <hyperlink ref="D7" r:id="rId24" xr:uid="{6CA69A82-E20A-4525-955A-629EFF7FED41}"/>
     <hyperlink ref="D8" r:id="rId25" xr:uid="{BF5198FE-BAFA-4C0E-925F-575EE5DDF14B}"/>
@@ -1829,8 +1861,9 @@
     <hyperlink ref="D16" r:id="rId33" xr:uid="{BF214671-2269-4A56-A738-777AE0D1A23B}"/>
     <hyperlink ref="D17" r:id="rId34" xr:uid="{2B655D3E-9F6D-4C4A-9A02-DAC1C011BC96}"/>
     <hyperlink ref="D18" r:id="rId35" xr:uid="{21ACE2EB-4E33-453D-BA93-6881E1705DE3}"/>
+    <hyperlink ref="D45" r:id="rId36" xr:uid="{CD3D7C1B-83D3-40EA-80B0-7847E235EC8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après modif version composants
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -503,9 +503,6 @@
     <t>https://dev.mysql.com/downloads/windows/installer/5.7.html</t>
   </si>
   <si>
-    <t>MySQL Connector/J  8.0.7-dmr</t>
-  </si>
-  <si>
     <t>8.0.7-dmr</t>
   </si>
   <si>
@@ -530,9 +527,6 @@
     <t>https://mvnrepository.com/artifact/postgresql/postgresql/9.1-901-1.jdbc4</t>
   </si>
   <si>
-    <t>PostgreSQL JDBC Driver 9.1-901-1.jdbc4</t>
-  </si>
-  <si>
     <t>9.1-901-1.jdbc4</t>
   </si>
   <si>
@@ -678,6 +672,12 @@
   </si>
   <si>
     <t>servlet-api 3.1</t>
+  </si>
+  <si>
+    <t>Driver MySQL Connector/J  8.0.7-dmr</t>
+  </si>
+  <si>
+    <t>Driver PostgreSQL JDBC Driver 9.1-901-1.jdbc4</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,7 +1187,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,170 +1209,170 @@
     </row>
     <row r="7" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="F16" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1384,16 +1384,16 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1623,7 +1623,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>47</v>
@@ -1637,36 +1637,36 @@
     </row>
     <row r="44" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1730,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>84</v>
@@ -1747,16 +1747,16 @@
         <v>48</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>83</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1764,16 +1764,16 @@
         <v>48</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E55" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="F55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1781,16 +1781,16 @@
         <v>48</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>94</v>
+        <v>143</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1801,13 +1801,13 @@
         <v>81</v>
       </c>
       <c r="D58" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="F58" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -1818,10 +1818,10 @@
         <v>75</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après chgt version composants
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -524,12 +524,6 @@
     <t>9.6.4</t>
   </si>
   <si>
-    <t>https://mvnrepository.com/artifact/postgresql/postgresql/9.1-901-1.jdbc4</t>
-  </si>
-  <si>
-    <t>9.1-901-1.jdbc4</t>
-  </si>
-  <si>
     <t>https://mvnrepository.com/artifact/org.apache.tomcat/tomcat-servlet-api/8.5.11</t>
   </si>
   <si>
@@ -674,10 +668,16 @@
     <t>Driver MySQL Connector/J  8.0.7-dmr</t>
   </si>
   <si>
-    <t>Driver PostgreSQL JDBC Driver 9.1-901-1.jdbc4</t>
-  </si>
-  <si>
     <t>Attention, la version de Maven utilisée (embarquée) dans Eclipse peut être différente</t>
+  </si>
+  <si>
+    <t>9.4.1212</t>
+  </si>
+  <si>
+    <t>Driver PostgreSQL JDBC postgresql-42.1.4.jar</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.postgresql/postgresql/42.1.4</t>
   </si>
 </sst>
 </file>
@@ -1092,8 +1092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,7 +1187,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,170 +1209,170 @@
     </row>
     <row r="7" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>106</v>
-      </c>
       <c r="F7" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>115</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>121</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="F15" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="F16" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="F17" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="F18" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1384,16 +1384,16 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>103</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1623,7 +1623,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>47</v>
@@ -1637,36 +1637,36 @@
     </row>
     <row r="44" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1730,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>84</v>
@@ -1747,7 +1747,7 @@
         <v>48</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>83</v>
@@ -1764,7 +1764,7 @@
         <v>48</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>90</v>
@@ -1784,13 +1784,13 @@
         <v>142</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après Hibernate 5.2.11
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="150">
   <si>
     <t>Version utilisée</t>
   </si>
@@ -431,12 +431,6 @@
     <t>ORM (object-relational mapping)</t>
   </si>
   <si>
-    <t>5.2.10.Final</t>
-  </si>
-  <si>
-    <t>https://mvnrepository.com/artifact/org.hibernate/hibernate-core/5.2.10.Final</t>
-  </si>
-  <si>
     <t>Tag Libraries</t>
   </si>
   <si>
@@ -488,9 +482,6 @@
     <t>JPA 2.1 (hibernate-jpa-2.1-api-1.0.0.Final-sources.jar)</t>
   </si>
   <si>
-    <t>Jboss Hibernate (Hibernate-core5.2.10.Final)</t>
-  </si>
-  <si>
     <t>UML 2.0</t>
   </si>
   <si>
@@ -665,19 +656,46 @@
     <t>servlet-api 3.1</t>
   </si>
   <si>
-    <t>Driver MySQL Connector/J  8.0.7-dmr</t>
-  </si>
-  <si>
     <t>Attention, la version de Maven utilisée (embarquée) dans Eclipse peut être différente</t>
   </si>
   <si>
-    <t>9.4.1212</t>
-  </si>
-  <si>
-    <t>Driver PostgreSQL JDBC postgresql-42.1.4.jar</t>
-  </si>
-  <si>
     <t>https://mvnrepository.com/artifact/org.postgresql/postgresql/42.1.4</t>
+  </si>
+  <si>
+    <t>Jboss Hibernate (Hibernate-core5.2.11.Final)</t>
+  </si>
+  <si>
+    <t>5.2.11.Final</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.hibernate/hibernate-core/5.2.11.Final</t>
+  </si>
+  <si>
+    <t>Driver MySQL Connector/J  8.0.7-dmr Type jdbc 4.2</t>
+  </si>
+  <si>
+    <t>Driver PostgreSQL JDBC postgresql-42.1.4.jar Type jdbc 4.2</t>
+  </si>
+  <si>
+    <t>42.1.4</t>
+  </si>
+  <si>
+    <t>Pool de connexion C3P0</t>
+  </si>
+  <si>
+    <t>hibernate-c3p0 5.2.11.Final</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.hibernate/hibernate-c3p0/5.2.11.Final</t>
+  </si>
+  <si>
+    <t>c3p0 0.9.5.2</t>
+  </si>
+  <si>
+    <t>0.9.5.2</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/com.mchange/c3p0/0.9.5.2</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:G59"/>
+  <dimension ref="B1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1187,7 +1205,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1209,170 +1227,170 @@
     </row>
     <row r="7" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1384,16 +1402,16 @@
         <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1527,36 +1545,36 @@
     </row>
     <row r="34" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="E35" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1565,19 +1583,19 @@
     </row>
     <row r="37" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="E37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="F37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1623,7 +1641,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>47</v>
@@ -1637,54 +1655,54 @@
     </row>
     <row r="44" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>52</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="C45" s="11" t="s">
-        <v>138</v>
-      </c>
       <c r="D45" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
@@ -1692,136 +1710,170 @@
         <v>60</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>61</v>
+        <v>139</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>144</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="10"/>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="10"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>96</v>
+        <v>141</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C57" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D58" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>86</v>
+    </row>
+    <row r="61" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1836,7 +1888,7 @@
     <hyperlink ref="D40" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="D41" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="D43" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D50" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D52" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="D30" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="D28" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="D48" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
@@ -1844,10 +1896,10 @@
     <hyperlink ref="D34" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="D35" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="D47" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="D53" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="D52" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="D55" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="D56" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="D55" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D54" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D57" r:id="rId21" location="windows" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="D58" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
     <hyperlink ref="D44" r:id="rId23" xr:uid="{94B18ED3-E673-44B7-AF22-1689CBC74A92}"/>
     <hyperlink ref="D7" r:id="rId24" xr:uid="{6CA69A82-E20A-4525-955A-629EFF7FED41}"/>
     <hyperlink ref="D8" r:id="rId25" xr:uid="{BF5198FE-BAFA-4C0E-925F-575EE5DDF14B}"/>
@@ -1862,8 +1914,10 @@
     <hyperlink ref="D17" r:id="rId34" xr:uid="{2B655D3E-9F6D-4C4A-9A02-DAC1C011BC96}"/>
     <hyperlink ref="D18" r:id="rId35" xr:uid="{21ACE2EB-4E33-453D-BA93-6881E1705DE3}"/>
     <hyperlink ref="D45" r:id="rId36" xr:uid="{CD3D7C1B-83D3-40EA-80B0-7847E235EC8A}"/>
+    <hyperlink ref="D49" r:id="rId37" xr:uid="{961E47A5-7366-4A5A-A389-85F13D48D722}"/>
+    <hyperlink ref="D50" r:id="rId38" xr:uid="{252C5999-0677-4C53-8079-791403160E3B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
COMMIT_DL_DOMICILE après Modif du POM
</commit_message>
<xml_diff>
--- a/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
+++ b/configuration_de_developpement/Configuration de développement/Versions_Technos_Composants.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="153">
   <si>
     <t>Version utilisée</t>
   </si>
@@ -696,13 +696,34 @@
   </si>
   <si>
     <t>https://mvnrepository.com/artifact/com.mchange/c3p0/0.9.5.2</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/org.apache.taglibs/taglibs-standard-impl/1.2.5</t>
+  </si>
+  <si>
+    <t>1.2.5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Apache Standard Taglib Implementation 1.2.5
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(complémentaire de jstl.1.2 pour Apache Tomcat)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -726,13 +747,33 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color theme="4" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -758,14 +799,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -773,24 +808,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1110,20 +1154,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="54.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="48.7109375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="19.5703125" style="1"/>
+    <col min="1" max="1" width="5.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="54.140625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="19.5703125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="2" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,743 +1180,756 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="6" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:7" s="4" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:7" s="6" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:7" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="6" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="2:7" s="4" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:7" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="6" t="s">
+    <row r="7" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="6" t="s">
+    <row r="8" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="6" t="s">
+    <row r="9" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C9" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="6" t="s">
+    <row r="10" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C10" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="6" t="s">
+    <row r="11" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="6" t="s">
+    <row r="12" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C12" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="6" t="s">
+    <row r="13" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="6" t="s">
+    <row r="14" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="6" t="s">
+    <row r="15" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="2:7" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="6" t="s">
+    <row r="16" spans="2:7" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C16" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="6" t="s">
+    <row r="17" spans="2:6" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="6" t="s">
+    <row r="18" spans="2:6" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="8"/>
-      <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+    <row r="19" spans="2:6" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:6" s="6" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="8"/>
-      <c r="E21" s="7"/>
+    <row r="21" spans="2:6" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="3"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="10"/>
-      <c r="D27" s="3"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="10"/>
-      <c r="D29" s="3"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="10"/>
-      <c r="D31" s="3"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="10"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="10"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="10"/>
-      <c r="D36" s="3"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" s="8" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="10"/>
-      <c r="D38" s="3"/>
+      <c r="B38" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="43" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="8" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="8" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="46" spans="2:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="48" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="49" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" s="8" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E50" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" s="8" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="10"/>
-      <c r="D53" s="3"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E57" s="5" t="s">
+      <c r="E57" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" s="8" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="60" spans="2:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E60" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="8" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="61" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E61" s="5" t="s">
+      <c r="E61" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" s="8" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1916,8 +1973,9 @@
     <hyperlink ref="D45" r:id="rId36" xr:uid="{CD3D7C1B-83D3-40EA-80B0-7847E235EC8A}"/>
     <hyperlink ref="D49" r:id="rId37" xr:uid="{961E47A5-7366-4A5A-A389-85F13D48D722}"/>
     <hyperlink ref="D50" r:id="rId38" xr:uid="{252C5999-0677-4C53-8079-791403160E3B}"/>
+    <hyperlink ref="D38" r:id="rId39" xr:uid="{0BA25C73-A201-410D-BA9B-4A155EFA0B83}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>